<commit_message>
eredménylevél küldés de nem jó
</commit_message>
<xml_diff>
--- a/KulturhazakMailcimesLista.xlsx
+++ b/KulturhazakMailcimesLista.xlsx
@@ -10,12 +10,11 @@
     <sheet name="talalt_kulturalis_intezmenyek_e" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1061" uniqueCount="1033">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1068" uniqueCount="1038">
   <si>
     <t>Intézmény neve</t>
   </si>
@@ -3116,6 +3115,21 @@
   </si>
   <si>
     <t>https://szentgrotkonyvtarvmk.hu/hu/munkatarsak/</t>
+  </si>
+  <si>
+    <t>Kami teszt intézménye</t>
+  </si>
+  <si>
+    <t>Illés Kálmán</t>
+  </si>
+  <si>
+    <t>illeskalman77@gmail.com</t>
+  </si>
+  <si>
+    <t>https://www.agoraszeged.hu/az-agora/munkatarsak</t>
+  </si>
+  <si>
+    <t>Agóra Szeged</t>
   </si>
 </sst>
 </file>
@@ -3990,10 +4004,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F319"/>
+  <dimension ref="A1:F321"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A292" workbookViewId="0">
-      <selection activeCell="D320" sqref="D320"/>
+    <sheetView tabSelected="1" topLeftCell="A306" workbookViewId="0">
+      <selection activeCell="A322" sqref="A322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7825,6 +7839,31 @@
       </c>
       <c r="D319" s="1" t="s">
         <v>1032</v>
+      </c>
+    </row>
+    <row r="320" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A320" t="s">
+        <v>1033</v>
+      </c>
+      <c r="B320" t="s">
+        <v>1034</v>
+      </c>
+      <c r="C320" s="1" t="s">
+        <v>1035</v>
+      </c>
+    </row>
+    <row r="321" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A321" t="s">
+        <v>1037</v>
+      </c>
+      <c r="B321" t="s">
+        <v>119</v>
+      </c>
+      <c r="C321" s="1" t="s">
+        <v>736</v>
+      </c>
+      <c r="D321" s="1" t="s">
+        <v>1036</v>
       </c>
     </row>
   </sheetData>
@@ -8138,7 +8177,7 @@
     <hyperlink ref="C282" r:id="rId307"/>
     <hyperlink ref="D282" r:id="rId308"/>
     <hyperlink ref="C283" r:id="rId309"/>
-    <hyperlink ref="D283"/>
+    <hyperlink ref="D283" display="https://www.google.com/url?sa=t&amp;source=web&amp;rct=j&amp;opi=89978449&amp;url=https://gyonk.hu/wp-content/uploads/2024/05/KT-2024_03_28-4_mell_Melleklet_Szolgaltatasi-terv-MuvHaz_2024.xlsx&amp;ved=2ahUKEwiKzPyb54mNAxXL8gIHHaPEKZwQFnoECDkQAQ&amp;usg=AOvVaw1X6D4Tv_q4mXjqEhso56"/>
     <hyperlink ref="C284" r:id="rId310"/>
     <hyperlink ref="D284" r:id="rId311"/>
     <hyperlink ref="C285" r:id="rId312"/>
@@ -8187,8 +8226,11 @@
     <hyperlink ref="C318" r:id="rId355"/>
     <hyperlink ref="C319" r:id="rId356"/>
     <hyperlink ref="D319" r:id="rId357"/>
+    <hyperlink ref="C320" r:id="rId358"/>
+    <hyperlink ref="D321" r:id="rId359"/>
+    <hyperlink ref="C321" r:id="rId360"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId358"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId361"/>
 </worksheet>
 </file>
</xml_diff>